<commit_message>
made table 52 in excel format
</commit_message>
<xml_diff>
--- a/data/T7-EXO/Trocas7-incubation-sta-profiles.xlsx
+++ b/data/T7-EXO/Trocas7-incubation-sta-profiles.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t xml:space="preserve">Expedition</t>
   </si>
@@ -98,15 +98,9 @@
     <t xml:space="preserve">BGA-PC µg/L</t>
   </si>
   <si>
-    <t xml:space="preserve">Press psi a</t>
-  </si>
-  <si>
     <t xml:space="preserve">Corrected surface Chl</t>
   </si>
   <si>
-    <t xml:space="preserve">Satinsky 50% depth (m)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Satinsky surface chl (May 2011) (ug/L)</t>
   </si>
   <si>
@@ -161,6 +155,27 @@
     <t xml:space="preserve">Depth_SMCP_11_7_J_13J101648_110716_155705_edit</t>
   </si>
   <si>
+    <t xml:space="preserve">Average channel depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% sampled depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% depth average DO (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% depth Turbidity (FNU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% depth Salinity (PSU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% depth pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface chlorophyll (µg/L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Long.</t>
   </si>
   <si>
@@ -168,18 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">Collection date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average channel depth (m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50% sampled depth (m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50% depth average DO (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface chlorophyll (µg/L)</t>
   </si>
   <si>
     <t xml:space="preserve">Macapá North</t>
@@ -202,14 +205,15 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -253,6 +257,13 @@
       <left/>
       <right/>
       <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -282,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,11 +318,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,15 +355,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
   </cols>
@@ -427,19 +450,13 @@
       <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>43559</v>
@@ -448,7 +465,7 @@
         <v>0.356319444444444</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>29.421</v>
@@ -484,7 +501,7 @@
         <v>34.3</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>52.27</v>
@@ -511,18 +528,15 @@
         <v>-1.31</v>
       </c>
       <c r="Z2" s="0" t="n">
-        <v>21.92</v>
-      </c>
-      <c r="AA2" s="0" t="n">
         <v>0.54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>43559</v>
@@ -531,7 +545,7 @@
         <v>0.356319444444444</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>29.421</v>
@@ -567,7 +581,7 @@
         <v>32.5</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>54.19</v>
@@ -594,18 +608,15 @@
         <v>-1.13</v>
       </c>
       <c r="Z3" s="0" t="n">
-        <v>1.167</v>
-      </c>
-      <c r="AA3" s="0" t="n">
         <v>0.824</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>43559</v>
@@ -614,7 +625,7 @@
         <v>0.543055555555555</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>40.264</v>
@@ -650,7 +661,7 @@
         <v>34.2</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R4" s="0" t="n">
         <v>68.91</v>
@@ -677,18 +688,15 @@
         <v>-1.29</v>
       </c>
       <c r="Z4" s="0" t="n">
-        <v>29.261</v>
-      </c>
-      <c r="AA4" s="0" t="n">
         <v>0.43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>43559</v>
@@ -697,7 +705,7 @@
         <v>0.543055555555555</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>40.264</v>
@@ -733,7 +741,7 @@
         <v>33.3</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R5" s="0" t="n">
         <v>43.38</v>
@@ -760,18 +768,15 @@
         <v>-1.28</v>
       </c>
       <c r="Z5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="0" t="n">
         <v>0.54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>43560</v>
@@ -780,7 +785,7 @@
         <v>0.468391203703704</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>28.337</v>
@@ -816,7 +821,7 @@
         <v>28.6</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R6" s="0" t="n">
         <v>40.28</v>
@@ -843,18 +848,15 @@
         <v>-1.3</v>
       </c>
       <c r="Z6" s="0" t="n">
-        <v>20.431</v>
-      </c>
-      <c r="AA6" s="0" t="n">
         <v>0.824</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>43560</v>
@@ -863,7 +865,7 @@
         <v>0.468391203703704</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>28.337</v>
@@ -899,7 +901,7 @@
         <v>28.7</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R7" s="0" t="n">
         <v>38.42</v>
@@ -926,18 +928,15 @@
         <v>-0.64</v>
       </c>
       <c r="Z7" s="0" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="AA7" s="0" t="n">
         <v>0.43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>42678</v>
@@ -946,7 +945,7 @@
         <v>0.566215277777778</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>31</v>
@@ -982,7 +981,7 @@
         <v>51.4</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R8" s="0" t="n">
         <v>36.12</v>
@@ -999,16 +998,16 @@
       <c r="Y8" s="0" t="n">
         <v>-1.23</v>
       </c>
-      <c r="AA8" s="0" t="n">
+      <c r="Z8" s="0" t="n">
         <v>0.45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>42679</v>
@@ -1017,7 +1016,7 @@
         <v>0.517314814814815</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>17</v>
@@ -1053,7 +1052,7 @@
         <v>47.4</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R9" s="0" t="n">
         <v>31.19</v>
@@ -1070,16 +1069,16 @@
       <c r="Y9" s="0" t="n">
         <v>-1.24</v>
       </c>
-      <c r="AA9" s="0" t="n">
+      <c r="Z9" s="0" t="n">
         <v>0.59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>42682</v>
@@ -1088,7 +1087,7 @@
         <v>0.560150462962963</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>24</v>
@@ -1124,33 +1123,21 @@
         <v>69.4</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="V10" s="0" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="W10" s="0" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="X10" s="0" t="n">
-        <v>-2.25</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>-2.25</v>
+        <v>30</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>1.67</v>
       </c>
       <c r="AA10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="0" t="n">
         <v>1.67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>42681</v>
@@ -1159,7 +1146,7 @@
         <v>0.542824074074074</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>25</v>
@@ -1195,24 +1182,12 @@
         <v>67.2</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="W11" s="0" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="X11" s="0" t="n">
-        <v>-2.2</v>
-      </c>
-      <c r="Y11" s="0" t="n">
-        <v>-2.2</v>
+        <v>30</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>1.99</v>
       </c>
       <c r="AA11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="0" t="n">
         <v>1.99</v>
       </c>
     </row>
@@ -1235,144 +1210,201 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="3" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="16.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="9" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="9" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="8.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="10.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="15" style="3" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>-51.051417</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>-0.083883</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>43563</v>
-      </c>
-      <c r="E2" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="C2" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="D2" s="5" t="n">
         <v>89.4</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>67.25</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>6.38</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>1.67</v>
       </c>
+      <c r="L2" s="6" t="n">
+        <v>-51.051417</v>
+      </c>
+      <c r="M2" s="6" t="n">
+        <v>-0.083883</v>
+      </c>
+      <c r="N2" s="7" t="n">
+        <v>43563</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>-50.62255</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>-0.156917</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>43563</v>
-      </c>
-      <c r="E3" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="C3" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="n">
+      <c r="D3" s="5" t="n">
         <v>86.5</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>65.26</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>6.31</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>1.99</v>
       </c>
+      <c r="L3" s="6" t="n">
+        <v>-50.62255</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>-0.156917</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <v>43563</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>91.5</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>68.91</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="L4" s="6" t="n">
         <v>-50.300127</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="M4" s="6" t="n">
         <v>0.741253</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="N4" s="7" t="n">
         <v>43559</v>
       </c>
-      <c r="E4" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="F4" s="3" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="n">
-        <v>91.5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="3" t="n">
+      <c r="D5" s="9" t="n">
+        <v>93</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>43.38</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="10" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="H5" s="10" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L5" s="6" t="n">
         <v>-49.428194</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="M5" s="6" t="n">
         <v>-0.173593</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="N5" s="7" t="n">
         <v>43560</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>